<commit_message>
Unit1.cpp - licence ELTEP, GALATEK
</commit_message>
<xml_diff>
--- a/DOC/kabiny_koncept/geometrie/caldan_web_radius.xlsx
+++ b/DOC/kabiny_koncept/geometrie/caldan_web_radius.xlsx
@@ -4,12 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="4755" windowHeight="1380"/>
+    <workbookView xWindow="120" yWindow="90" windowWidth="4755" windowHeight="1380" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Podlahový" sheetId="1" r:id="rId1"/>
     <sheet name="Podvěsný" sheetId="2" r:id="rId2"/>
-    <sheet name="List3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
@@ -242,18 +241,12 @@
       <charset val="238"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -278,17 +271,16 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hypertextový odkaz" xfId="1" builtinId="8"/>
@@ -593,8 +585,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -608,24 +600,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5" t="s">
+      <c r="B1" s="3"/>
+      <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5" t="s">
+      <c r="D1" s="3"/>
+      <c r="E1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" s="5" t="s">
+      <c r="F1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="3" t="s">
         <v>6</v>
       </c>
     </row>
@@ -705,7 +697,7 @@
       <c r="G5" t="s">
         <v>11</v>
       </c>
-      <c r="H5" s="3">
+      <c r="H5" s="2">
         <v>1000</v>
       </c>
     </row>
@@ -725,34 +717,34 @@
       <c r="G6" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="3">
+      <c r="H6" s="2">
         <v>1000</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5" t="s">
+      <c r="B9" s="3"/>
+      <c r="C9" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5" t="s">
+      <c r="D9" s="3"/>
+      <c r="E9" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="G9" s="5" t="s">
+      <c r="F9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G9" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="H9" s="5" t="s">
+      <c r="H9" s="3" t="s">
         <v>6</v>
       </c>
     </row>
@@ -774,29 +766,29 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="1" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5" t="s">
+      <c r="B13" s="3"/>
+      <c r="C13" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5" t="s">
+      <c r="D13" s="3"/>
+      <c r="E13" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F13" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="G13" s="5" t="s">
+      <c r="F13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G13" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="H13" s="5" t="s">
+      <c r="H13" s="3" t="s">
         <v>6</v>
       </c>
     </row>
@@ -818,29 +810,29 @@
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="1" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5" t="s">
+      <c r="B17" s="3"/>
+      <c r="C17" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5" t="s">
+      <c r="D17" s="3"/>
+      <c r="E17" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F17" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="G17" s="5" t="s">
+      <c r="F17" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G17" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="H17" s="5" t="s">
+      <c r="H17" s="3" t="s">
         <v>6</v>
       </c>
     </row>
@@ -854,7 +846,7 @@
       <c r="F18" t="s">
         <v>7</v>
       </c>
-      <c r="G18" s="3">
+      <c r="G18" s="2">
         <v>30</v>
       </c>
       <c r="H18" t="s">
@@ -862,29 +854,29 @@
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="1" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
+      <c r="A21" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5" t="s">
+      <c r="B21" s="3"/>
+      <c r="C21" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5" t="s">
+      <c r="D21" s="3"/>
+      <c r="E21" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="F21" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="G21" s="5" t="s">
+      <c r="F21" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G21" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="H21" s="5" t="s">
+      <c r="H21" s="3" t="s">
         <v>6</v>
       </c>
     </row>
@@ -898,7 +890,7 @@
       <c r="F22" t="s">
         <v>28</v>
       </c>
-      <c r="G22" s="3" t="s">
+      <c r="G22" s="2" t="s">
         <v>29</v>
       </c>
       <c r="H22" t="s">
@@ -906,29 +898,29 @@
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
+      <c r="A23" s="1" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="5" t="s">
+      <c r="A25" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5" t="s">
+      <c r="B25" s="3"/>
+      <c r="C25" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5" t="s">
+      <c r="D25" s="3"/>
+      <c r="E25" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="F25" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="G25" s="5" t="s">
+      <c r="F25" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G25" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="H25" s="5" t="s">
+      <c r="H25" s="3" t="s">
         <v>6</v>
       </c>
     </row>
@@ -950,29 +942,29 @@
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
+      <c r="A27" s="1" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="5" t="s">
+      <c r="A29" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B29" s="5"/>
-      <c r="C29" s="5" t="s">
+      <c r="B29" s="3"/>
+      <c r="C29" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5" t="s">
+      <c r="D29" s="3"/>
+      <c r="E29" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="F29" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="G29" s="5" t="s">
+      <c r="F29" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G29" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="H29" s="5" t="s">
+      <c r="H29" s="3" t="s">
         <v>6</v>
       </c>
     </row>
@@ -994,29 +986,29 @@
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
+      <c r="A31" s="1" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="5" t="s">
+      <c r="A33" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B33" s="5"/>
-      <c r="C33" s="5" t="s">
+      <c r="B33" s="3"/>
+      <c r="C33" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D33" s="5"/>
-      <c r="E33" s="5" t="s">
+      <c r="D33" s="3"/>
+      <c r="E33" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="F33" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="G33" s="5" t="s">
+      <c r="F33" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G33" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="H33" s="5" t="s">
+      <c r="H33" s="3" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1038,29 +1030,29 @@
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
+      <c r="A35" s="1" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="5" t="s">
+      <c r="A37" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B37" s="5"/>
-      <c r="C37" s="5" t="s">
+      <c r="B37" s="3"/>
+      <c r="C37" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D37" s="5"/>
-      <c r="E37" s="5" t="s">
+      <c r="D37" s="3"/>
+      <c r="E37" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="F37" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="G37" s="5" t="s">
+      <c r="F37" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G37" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="H37" s="5" t="s">
+      <c r="H37" s="3" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1082,29 +1074,29 @@
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
+      <c r="A39" s="1" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="5" t="s">
+      <c r="A41" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B41" s="5"/>
-      <c r="C41" s="5" t="s">
+      <c r="B41" s="3"/>
+      <c r="C41" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D41" s="5"/>
-      <c r="E41" s="5" t="s">
+      <c r="D41" s="3"/>
+      <c r="E41" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="F41" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="G41" s="5" t="s">
+      <c r="F41" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G41" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="H41" s="5" t="s">
+      <c r="H41" s="3" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1126,7 +1118,7 @@
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="2" t="s">
+      <c r="A43" s="1" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1157,8 +1149,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1171,24 +1163,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="3"/>
+      <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1" t="s">
+      <c r="D1" s="3"/>
+      <c r="E1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="F1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="3" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1210,29 +1202,29 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1" t="s">
+      <c r="B5" s="3"/>
+      <c r="C5" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1" t="s">
+      <c r="D5" s="3"/>
+      <c r="E5" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G5" s="1" t="s">
+      <c r="F5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="H5" s="1" t="s">
+      <c r="H5" s="3" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1337,29 +1329,29 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="1" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1" t="s">
+      <c r="B13" s="3"/>
+      <c r="C13" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1" t="s">
+      <c r="D13" s="3"/>
+      <c r="E13" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F13" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G13" s="1" t="s">
+      <c r="F13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G13" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="H13" s="1" t="s">
+      <c r="H13" s="3" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1439,7 +1431,7 @@
       <c r="G17" t="s">
         <v>11</v>
       </c>
-      <c r="H17" s="3">
+      <c r="H17" s="2">
         <v>1000</v>
       </c>
     </row>
@@ -1459,34 +1451,34 @@
       <c r="G18" t="s">
         <v>11</v>
       </c>
-      <c r="H18" s="3">
+      <c r="H18" s="2">
         <v>1000</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="1" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+      <c r="A21" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1" t="s">
+      <c r="B21" s="3"/>
+      <c r="C21" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1" t="s">
+      <c r="D21" s="3"/>
+      <c r="E21" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F21" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G21" s="1" t="s">
+      <c r="F21" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G21" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="H21" s="1" t="s">
+      <c r="H21" s="3" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1503,35 +1495,35 @@
       <c r="G22" t="s">
         <v>19</v>
       </c>
-      <c r="H22" s="3">
+      <c r="H22" s="2">
         <v>2500</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
+      <c r="A23" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="H23" s="3"/>
+      <c r="H23" s="2"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H24" s="3"/>
+      <c r="H24" s="2"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
+      <c r="A25" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1" t="s">
+      <c r="B25" s="3"/>
+      <c r="C25" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1" t="s">
+      <c r="D25" s="3"/>
+      <c r="E25" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F25" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G25" s="1" t="s">
+      <c r="F25" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G25" s="3" t="s">
         <v>24</v>
       </c>
       <c r="H25" s="4" t="s">
@@ -1551,34 +1543,34 @@
       <c r="G26" t="s">
         <v>53</v>
       </c>
-      <c r="H26" s="3">
+      <c r="H26" s="2">
         <v>2500</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
+      <c r="A27" s="1" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
+      <c r="A29" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1" t="s">
+      <c r="B29" s="3"/>
+      <c r="C29" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1" t="s">
+      <c r="D29" s="3"/>
+      <c r="E29" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F29" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G29" s="1" t="s">
+      <c r="F29" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G29" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="H29" s="1" t="s">
+      <c r="H29" s="3" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1589,7 +1581,7 @@
       <c r="E30" t="s">
         <v>9</v>
       </c>
-      <c r="F30" s="3">
+      <c r="F30" s="2">
         <v>1500</v>
       </c>
       <c r="G30" t="s">
@@ -1614,16 +1606,4 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
katalog dopravniku - přidání print screenu z tisplu
</commit_message>
<xml_diff>
--- a/DOC/kabiny_koncept/geometrie/caldan_web_radius.xlsx
+++ b/DOC/kabiny_koncept/geometrie/caldan_web_radius.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="90" windowWidth="4755" windowHeight="1380"/>
@@ -9,14 +9,14 @@
   <sheets>
     <sheet name="Podlahový" sheetId="1" r:id="rId1"/>
     <sheet name="Podvěsný" sheetId="2" r:id="rId2"/>
-    <sheet name="List3" sheetId="3" r:id="rId3"/>
+    <sheet name="screen aplikace" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="60">
   <si>
     <t>Rozteč palců</t>
   </si>
@@ -46,9 +46,6 @@
   </si>
   <si>
     <t>90;45;30;15</t>
-  </si>
-  <si>
-    <t>Vertikální oblouky</t>
   </si>
   <si>
     <t>15;30;45;90</t>
@@ -216,8 +213,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -292,7 +289,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hypertextový odkaz" xfId="1" builtinId="8"/>
-    <cellStyle name="Normální" xfId="0" builtinId="0"/>
+    <cellStyle name="normální" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -304,8 +301,60 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1025" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="190500"/>
+          <a:ext cx="10201275" cy="4000500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motiv systému Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motiv sady Office">
   <a:themeElements>
     <a:clrScheme name="Kancelář">
       <a:dk1>
@@ -379,7 +428,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -414,7 +462,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Kancelář">
@@ -590,14 +637,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
@@ -607,9 +654,9 @@
     <col min="8" max="8" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="A1" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="5" t="s">
@@ -617,24 +664,24 @@
       </c>
       <c r="D1" s="5"/>
       <c r="E1" s="5" t="s">
-        <v>22</v>
+        <v>58</v>
       </c>
       <c r="F1" s="5" t="s">
         <v>6</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>10</v>
+        <v>59</v>
       </c>
       <c r="H1" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E2" t="s">
         <v>9</v>
@@ -643,18 +690,18 @@
         <v>8</v>
       </c>
       <c r="G2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E3" t="s">
         <v>9</v>
@@ -663,18 +710,18 @@
         <v>8</v>
       </c>
       <c r="G3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E4" t="s">
         <v>9</v>
@@ -683,18 +730,18 @@
         <v>8</v>
       </c>
       <c r="G4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E5" t="s">
         <v>9</v>
@@ -703,18 +750,18 @@
         <v>7</v>
       </c>
       <c r="G5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H5" s="3">
         <v>1000</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E6" t="s">
         <v>9</v>
@@ -723,20 +770,20 @@
         <v>7</v>
       </c>
       <c r="G6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H6" s="3">
         <v>1000</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8">
       <c r="A7" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="5" t="s">
@@ -744,21 +791,21 @@
       </c>
       <c r="D9" s="5"/>
       <c r="E9" s="5" t="s">
-        <v>22</v>
+        <v>58</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>6</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>24</v>
+        <v>59</v>
       </c>
       <c r="H9" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8">
       <c r="C10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E10" t="s">
         <v>9</v>
@@ -767,20 +814,20 @@
         <v>8</v>
       </c>
       <c r="G10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H10">
         <v>1000</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8">
       <c r="A11" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
       <c r="A13" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B13" s="5"/>
       <c r="C13" s="5" t="s">
@@ -788,43 +835,43 @@
       </c>
       <c r="D13" s="5"/>
       <c r="E13" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="C14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" t="s">
+        <v>7</v>
+      </c>
+      <c r="G14" t="s">
+        <v>18</v>
+      </c>
+      <c r="H14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F13" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="G13" s="5" t="s">
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="5" t="s">
         <v>24</v>
-      </c>
-      <c r="H13" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C14" t="s">
-        <v>18</v>
-      </c>
-      <c r="E14" t="s">
-        <v>9</v>
-      </c>
-      <c r="F14" t="s">
-        <v>7</v>
-      </c>
-      <c r="G14" t="s">
-        <v>19</v>
-      </c>
-      <c r="H14" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
-        <v>25</v>
       </c>
       <c r="B17" s="5"/>
       <c r="C17" s="5" t="s">
@@ -832,21 +879,21 @@
       </c>
       <c r="D17" s="5"/>
       <c r="E17" s="5" t="s">
-        <v>22</v>
+        <v>58</v>
       </c>
       <c r="F17" s="5" t="s">
         <v>6</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>24</v>
+        <v>59</v>
       </c>
       <c r="H17" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8">
       <c r="C18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E18" t="s">
         <v>9</v>
@@ -858,17 +905,17 @@
         <v>30</v>
       </c>
       <c r="H18" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
       <c r="A19" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
       <c r="A21" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B21" s="5"/>
       <c r="C21" s="5" t="s">
@@ -876,43 +923,43 @@
       </c>
       <c r="D21" s="5"/>
       <c r="E21" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F21" s="5" t="s">
         <v>6</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H21" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8">
       <c r="C22" t="s">
+        <v>26</v>
+      </c>
+      <c r="E22" t="s">
+        <v>9</v>
+      </c>
+      <c r="F22" t="s">
         <v>27</v>
       </c>
-      <c r="E22" t="s">
-        <v>9</v>
-      </c>
-      <c r="F22" t="s">
+      <c r="G22" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G22" s="3" t="s">
+      <c r="H22" t="s">
         <v>29</v>
       </c>
-      <c r="H22" t="s">
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8">
       <c r="A25" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B25" s="5"/>
       <c r="C25" s="5" t="s">
@@ -920,43 +967,43 @@
       </c>
       <c r="D25" s="5"/>
       <c r="E25" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G25" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="F25" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="G25" s="5" t="s">
-        <v>60</v>
-      </c>
       <c r="H25" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8">
       <c r="C26" t="s">
+        <v>17</v>
+      </c>
+      <c r="E26" t="s">
+        <v>9</v>
+      </c>
+      <c r="F26" t="s">
+        <v>7</v>
+      </c>
+      <c r="G26" t="s">
         <v>18</v>
       </c>
-      <c r="E26" t="s">
-        <v>9</v>
-      </c>
-      <c r="F26" t="s">
-        <v>7</v>
-      </c>
-      <c r="G26" t="s">
-        <v>19</v>
-      </c>
       <c r="H26" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
       <c r="A27" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="A29" s="5" t="s">
         <v>34</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="5" t="s">
-        <v>35</v>
       </c>
       <c r="B29" s="5"/>
       <c r="C29" s="5" t="s">
@@ -964,43 +1011,43 @@
       </c>
       <c r="D29" s="5"/>
       <c r="E29" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G29" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="F29" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="G29" s="5" t="s">
-        <v>60</v>
-      </c>
       <c r="H29" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8">
       <c r="C30" t="s">
+        <v>17</v>
+      </c>
+      <c r="E30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F30" t="s">
+        <v>7</v>
+      </c>
+      <c r="G30" t="s">
         <v>18</v>
       </c>
-      <c r="E30" t="s">
-        <v>9</v>
-      </c>
-      <c r="F30" t="s">
-        <v>7</v>
-      </c>
-      <c r="G30" t="s">
-        <v>19</v>
-      </c>
       <c r="H30" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
       <c r="A31" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
       <c r="A33" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B33" s="5"/>
       <c r="C33" s="5" t="s">
@@ -1008,43 +1055,43 @@
       </c>
       <c r="D33" s="5"/>
       <c r="E33" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G33" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="F33" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="G33" s="5" t="s">
-        <v>60</v>
-      </c>
       <c r="H33" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8">
       <c r="C34" t="s">
+        <v>17</v>
+      </c>
+      <c r="E34" t="s">
+        <v>9</v>
+      </c>
+      <c r="F34" t="s">
+        <v>7</v>
+      </c>
+      <c r="G34" t="s">
         <v>18</v>
-      </c>
-      <c r="E34" t="s">
-        <v>9</v>
-      </c>
-      <c r="F34" t="s">
-        <v>7</v>
-      </c>
-      <c r="G34" t="s">
-        <v>19</v>
       </c>
       <c r="H34">
         <v>1000</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8">
       <c r="A35" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8">
       <c r="A37" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B37" s="5"/>
       <c r="C37" s="5" t="s">
@@ -1052,43 +1099,43 @@
       </c>
       <c r="D37" s="5"/>
       <c r="E37" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G37" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="F37" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="G37" s="5" t="s">
-        <v>60</v>
-      </c>
       <c r="H37" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8">
       <c r="C38" t="s">
+        <v>26</v>
+      </c>
+      <c r="E38" t="s">
+        <v>9</v>
+      </c>
+      <c r="F38" t="s">
         <v>27</v>
       </c>
-      <c r="E38" t="s">
-        <v>9</v>
-      </c>
-      <c r="F38" t="s">
-        <v>28</v>
-      </c>
       <c r="G38" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H38" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8">
       <c r="A39" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8">
       <c r="A41" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B41" s="5"/>
       <c r="C41" s="5" t="s">
@@ -1096,43 +1143,43 @@
       </c>
       <c r="D41" s="5"/>
       <c r="E41" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="F41" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G41" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="F41" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="G41" s="5" t="s">
-        <v>60</v>
-      </c>
       <c r="H41" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8">
       <c r="C42" t="s">
+        <v>26</v>
+      </c>
+      <c r="E42" t="s">
+        <v>9</v>
+      </c>
+      <c r="F42" t="s">
         <v>27</v>
       </c>
-      <c r="E42" t="s">
-        <v>9</v>
-      </c>
-      <c r="F42" t="s">
-        <v>28</v>
-      </c>
       <c r="G42" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H42" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8">
       <c r="A43" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8">
       <c r="A45" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -1154,14 +1201,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="28" bestFit="1" customWidth="1"/>
@@ -1170,9 +1217,9 @@
     <col min="8" max="8" width="8.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1" t="s">
@@ -1180,43 +1227,43 @@
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="C2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
         <v>43</v>
       </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="G2" t="s">
-        <v>43</v>
-      </c>
-      <c r="H2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
@@ -1224,24 +1271,24 @@
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E6" t="s">
         <v>9</v>
@@ -1250,18 +1297,18 @@
         <v>8</v>
       </c>
       <c r="G6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
         <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E7" t="s">
         <v>9</v>
@@ -1270,18 +1317,18 @@
         <v>8</v>
       </c>
       <c r="G7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
         <v>3</v>
       </c>
       <c r="C8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E8" t="s">
         <v>9</v>
@@ -1290,18 +1337,18 @@
         <v>8</v>
       </c>
       <c r="G8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
         <v>4</v>
       </c>
       <c r="C9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E9" t="s">
         <v>9</v>
@@ -1310,18 +1357,18 @@
         <v>7</v>
       </c>
       <c r="G9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H9">
         <v>1000</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8">
       <c r="A10" t="s">
         <v>5</v>
       </c>
       <c r="C10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E10" t="s">
         <v>9</v>
@@ -1330,20 +1377,20 @@
         <v>7</v>
       </c>
       <c r="G10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H10">
         <v>1000</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8">
       <c r="A11" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
       <c r="A13" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1" t="s">
@@ -1351,24 +1398,24 @@
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8">
       <c r="A14" t="s">
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E14" t="s">
         <v>9</v>
@@ -1377,18 +1424,18 @@
         <v>8</v>
       </c>
       <c r="G14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H14" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8">
       <c r="A15" t="s">
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E15" t="s">
         <v>9</v>
@@ -1397,18 +1444,18 @@
         <v>8</v>
       </c>
       <c r="G15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H15" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8">
       <c r="A16" t="s">
         <v>3</v>
       </c>
       <c r="C16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E16" t="s">
         <v>9</v>
@@ -1417,18 +1464,18 @@
         <v>8</v>
       </c>
       <c r="G16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H16" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8">
       <c r="A17" t="s">
         <v>4</v>
       </c>
       <c r="C17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E17" t="s">
         <v>9</v>
@@ -1437,18 +1484,18 @@
         <v>7</v>
       </c>
       <c r="G17" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H17" s="3">
         <v>1000</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8">
       <c r="A18" t="s">
         <v>5</v>
       </c>
       <c r="C18" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E18" t="s">
         <v>9</v>
@@ -1457,20 +1504,20 @@
         <v>7</v>
       </c>
       <c r="G18" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H18" s="3">
         <v>1000</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8">
       <c r="A19" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
       <c r="A21" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1" t="s">
@@ -1478,47 +1525,47 @@
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H21" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8">
       <c r="C22" t="s">
+        <v>17</v>
+      </c>
+      <c r="E22" t="s">
+        <v>9</v>
+      </c>
+      <c r="F22" t="s">
+        <v>7</v>
+      </c>
+      <c r="G22" t="s">
         <v>18</v>
-      </c>
-      <c r="E22" t="s">
-        <v>9</v>
-      </c>
-      <c r="F22" t="s">
-        <v>7</v>
-      </c>
-      <c r="G22" t="s">
-        <v>19</v>
       </c>
       <c r="H22" s="3">
         <v>2500</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8">
       <c r="A23" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H23" s="3"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8">
       <c r="H24" s="3"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8">
       <c r="A25" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B25" s="1"/>
       <c r="C25" s="1" t="s">
@@ -1526,21 +1573,21 @@
       </c>
       <c r="D25" s="1"/>
       <c r="E25" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H25" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8">
       <c r="C26" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E26" t="s">
         <v>9</v>
@@ -1549,20 +1596,20 @@
         <v>7</v>
       </c>
       <c r="G26" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H26" s="3">
         <v>2500</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8">
       <c r="A27" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
       <c r="A29" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B29" s="1"/>
       <c r="C29" s="1" t="s">
@@ -1570,21 +1617,21 @@
       </c>
       <c r="D29" s="1"/>
       <c r="E29" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>6</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H29" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8">
       <c r="C30" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E30" t="s">
         <v>9</v>
@@ -1593,15 +1640,15 @@
         <v>1500</v>
       </c>
       <c r="G30" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H30" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
       <c r="A32" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -1617,13 +1664,16 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="S14" sqref="S14"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>